<commit_message>
Create class add table in base
</commit_message>
<xml_diff>
--- a/excel/src.xlsx
+++ b/excel/src.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ывфы</t>
   </si>
@@ -45,10 +45,13 @@
     <t>quentity</t>
   </si>
   <si>
-    <t>delivery_date</t>
-  </si>
-  <si>
     <t>Client.Client_No</t>
+  </si>
+  <si>
+    <t>Goods.Goods_No</t>
+  </si>
+  <si>
+    <t>Order.Goods_Name</t>
   </si>
 </sst>
 </file>
@@ -84,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -387,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,9 +405,11 @@
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,14 +417,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -435,16 +441,25 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
+      <c r="F4" s="1">
+        <v>42323</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>